<commit_message>
update on matching and port-choice (installation and om)
</commit_message>
<xml_diff>
--- a/src/databases/Installation_Order.xlsx
+++ b/src/databases/Installation_Order.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="449" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="InstallationOrder" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>id</t>
   </si>
@@ -26,22 +26,7 @@
     <t>Default Order</t>
   </si>
   <si>
-    <t>installation of export static cables</t>
-  </si>
-  <si>
-    <t>installation of array static cables</t>
-  </si>
-  <si>
-    <t>installation of dynamic cables</t>
-  </si>
-  <si>
-    <t>installation of collection points</t>
-  </si>
-  <si>
-    <t>installation of external cable protection</t>
-  </si>
-  <si>
-    <t>Installation of Foundations</t>
+    <t>Installation of Electrical Connection</t>
   </si>
   <si>
     <t>Installation of Moorings</t>
@@ -169,17 +154,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
-      <selection activeCell="C17" activeCellId="0" pane="topLeft" sqref="C17"/>
+      <selection activeCell="C4" activeCellId="0" pane="topLeft" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.0823529411765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8862745098039"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.6196078431373"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.60392156862745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1686274509804"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.2117647058823"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.1058823529412"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.67843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="1">
@@ -193,92 +178,37 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="2">
       <c r="A2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3" t="n">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="3">
+      <c r="A3" s="3" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="3">
-      <c r="A3" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="4">
+      <c r="A4" s="4" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="4">
-      <c r="A4" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="3" t="n">
         <v>3</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="5">
-      <c r="A5" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="3" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="6">
-      <c r="A6" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="7">
-      <c r="A7" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="3" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="8">
-      <c r="A8" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="3" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="9">
-      <c r="A9" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="3" t="n">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>